<commit_message>
Poster Table and Charts
</commit_message>
<xml_diff>
--- a/results/experiment1/sokwholes-output-fixedcsv.xlsx
+++ b/results/experiment1/sokwholes-output-fixedcsv.xlsx
@@ -1,20 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangzijiang/Dropbox (Davidson College)/Davidson/04 4th Year/CSC370 - Machine Reasoning/SokobanSolver_MR_Final/results/experiment1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5DD7CD-722C-6040-8DDE-008DF2A7335D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="2380" yWindow="980" windowWidth="24240" windowHeight="17020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sokwholes-output-fixedcsv" sheetId="1" r:id="rId1"/>
+    <sheet name="Result" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="143">
   <si>
     <t>Puzzle Name</t>
   </si>
@@ -376,14 +392,133 @@
     <t>Avg Generated</t>
   </si>
   <si>
-    <t>Total Explored</t>
+    <t>Solved in 2 Mins</t>
+  </si>
+  <si>
+    <t>Nodes in Fringe</t>
+  </si>
+  <si>
+    <t>Nodes Explored</t>
+  </si>
+  <si>
+    <t>Duration (secs)</t>
+  </si>
+  <si>
+    <t>Solution Length</t>
+  </si>
+  <si>
+    <t>Method - Heuristics - Bound Increment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solved % </t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>IDA* - Manhattan - Fixed (1)</t>
+  </si>
+  <si>
+    <t>IDA* - Manhattan - Fixed (4)</t>
+  </si>
+  <si>
+    <t>IDA* - Manhattan - Dynamic</t>
+  </si>
+  <si>
+    <t>IDA* - Euclidean - Fixed (1)</t>
+  </si>
+  <si>
+    <t>IDA* - Euclidean - Fixed (4)</t>
+  </si>
+  <si>
+    <t>IDA* - Euclidean - Dynamic</t>
+  </si>
+  <si>
+    <t>Fringe</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>explored</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>Solution length</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 1: Comparisons of Performances by BFS and IDA* on 30 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Microban</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Puzzles</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 2: Comparisons of Performances by BFS and IDA* on 30 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sokowhole</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Puzzles</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -518,8 +653,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,8 +867,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -815,6 +995,246 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -861,9 +1281,65 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="25" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="30" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -921,6 +1397,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A609C2FF-A517-B14E-BED0-3FEE4FA33E82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="812800"/>
+          <a:ext cx="5943600" cy="5715000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1212,26 +1737,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K180"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="F146" workbookViewId="0">
+      <selection activeCell="T165" sqref="T165:U171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1265,8 +1790,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1300,8 +1828,12 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>LEN(K2)/2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1335,8 +1867,12 @@
       <c r="K3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L66" si="0">LEN(K3)/2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1370,8 +1906,12 @@
       <c r="K4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1405,8 +1945,12 @@
       <c r="K5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1440,8 +1984,12 @@
       <c r="K6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1475,8 +2023,12 @@
       <c r="K7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1510,8 +2062,12 @@
       <c r="K8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1545,8 +2101,12 @@
       <c r="K9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1580,8 +2140,12 @@
       <c r="K10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1615,8 +2179,12 @@
       <c r="K11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1650,8 +2218,12 @@
       <c r="K12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1685,8 +2257,12 @@
       <c r="K13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1720,8 +2296,12 @@
       <c r="K14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1755,8 +2335,12 @@
       <c r="K15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1790,8 +2374,12 @@
       <c r="K16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1825,8 +2413,12 @@
       <c r="K17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1860,8 +2452,12 @@
       <c r="K18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1895,8 +2491,12 @@
       <c r="K19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1930,8 +2530,12 @@
       <c r="K20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1965,8 +2569,12 @@
       <c r="K21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2000,8 +2608,12 @@
       <c r="K22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2035,8 +2647,12 @@
       <c r="K23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2070,8 +2686,12 @@
       <c r="K24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2105,8 +2725,12 @@
       <c r="K25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2140,8 +2764,12 @@
       <c r="K26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2175,8 +2803,12 @@
       <c r="K27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2210,8 +2842,12 @@
       <c r="K28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2245,8 +2881,12 @@
       <c r="K29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2280,8 +2920,12 @@
       <c r="K30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -2315,8 +2959,12 @@
       <c r="K31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2350,8 +2998,12 @@
       <c r="K32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -2385,8 +3037,12 @@
       <c r="K33" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -2420,8 +3076,12 @@
       <c r="K34" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -2455,8 +3115,12 @@
       <c r="K35" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>28</v>
       </c>
@@ -2490,8 +3154,12 @@
       <c r="K36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -2525,8 +3193,12 @@
       <c r="K37" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -2560,8 +3232,12 @@
       <c r="K38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -2595,8 +3271,12 @@
       <c r="K39" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -2630,8 +3310,12 @@
       <c r="K40" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -2665,8 +3349,12 @@
       <c r="K41" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -2700,8 +3388,12 @@
       <c r="K42" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2735,8 +3427,12 @@
       <c r="K43" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -2770,8 +3466,12 @@
       <c r="K44" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -2805,8 +3505,12 @@
       <c r="K45" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -2840,8 +3544,12 @@
       <c r="K46" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -2875,8 +3583,12 @@
       <c r="K47" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -2910,8 +3622,12 @@
       <c r="K48" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -2945,8 +3661,12 @@
       <c r="K49" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -2980,8 +3700,12 @@
       <c r="K50" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -3015,8 +3739,12 @@
       <c r="K51" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -3050,8 +3778,12 @@
       <c r="K52" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -3085,8 +3817,12 @@
       <c r="K53" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -3120,8 +3856,12 @@
       <c r="K54" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -3155,8 +3895,12 @@
       <c r="K55" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>35</v>
       </c>
@@ -3190,8 +3934,12 @@
       <c r="K56" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -3225,8 +3973,12 @@
       <c r="K57" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -3260,8 +4012,12 @@
       <c r="K58" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -3295,8 +4051,12 @@
       <c r="K59" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>38</v>
       </c>
@@ -3330,8 +4090,12 @@
       <c r="K60" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -3365,8 +4129,12 @@
       <c r="K61" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -3400,8 +4168,12 @@
       <c r="K62" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>38</v>
       </c>
@@ -3435,8 +4207,12 @@
       <c r="K63" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -3470,8 +4246,12 @@
       <c r="K64" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>40</v>
       </c>
@@ -3505,8 +4285,12 @@
       <c r="K65" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>40</v>
       </c>
@@ -3540,8 +4324,12 @@
       <c r="K66" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>40</v>
       </c>
@@ -3575,8 +4363,12 @@
       <c r="K67" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <f t="shared" ref="L67:L130" si="1">LEN(K67)/2</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -3610,8 +4402,12 @@
       <c r="K68" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>40</v>
       </c>
@@ -3645,8 +4441,12 @@
       <c r="K69" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>40</v>
       </c>
@@ -3680,8 +4480,12 @@
       <c r="K70" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>40</v>
       </c>
@@ -3715,8 +4519,12 @@
       <c r="K71" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>43</v>
       </c>
@@ -3750,8 +4558,12 @@
       <c r="K72" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>43</v>
       </c>
@@ -3785,8 +4597,12 @@
       <c r="K73" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>43</v>
       </c>
@@ -3820,8 +4636,12 @@
       <c r="K74" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -3855,8 +4675,12 @@
       <c r="K75" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -3890,8 +4714,12 @@
       <c r="K76" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>43</v>
       </c>
@@ -3925,8 +4753,12 @@
       <c r="K77" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>43</v>
       </c>
@@ -3960,8 +4792,12 @@
       <c r="K78" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -3995,8 +4831,12 @@
       <c r="K79" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -4030,8 +4870,12 @@
       <c r="K80" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -4065,8 +4909,12 @@
       <c r="K81" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -4100,8 +4948,12 @@
       <c r="K82" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -4135,8 +4987,12 @@
       <c r="K83" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -4170,8 +5026,12 @@
       <c r="K84" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -4205,8 +5065,12 @@
       <c r="K85" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>50</v>
       </c>
@@ -4240,8 +5104,12 @@
       <c r="K86" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>50</v>
       </c>
@@ -4275,8 +5143,12 @@
       <c r="K87" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>50</v>
       </c>
@@ -4310,8 +5182,12 @@
       <c r="K88" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>50</v>
       </c>
@@ -4345,8 +5221,12 @@
       <c r="K89" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>50</v>
       </c>
@@ -4380,8 +5260,12 @@
       <c r="K90" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>50</v>
       </c>
@@ -4415,8 +5299,12 @@
       <c r="K91" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>50</v>
       </c>
@@ -4450,8 +5338,12 @@
       <c r="K92" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L92">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>54</v>
       </c>
@@ -4485,8 +5377,12 @@
       <c r="K93" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L93">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>54</v>
       </c>
@@ -4520,8 +5416,12 @@
       <c r="K94" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L94">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>54</v>
       </c>
@@ -4555,8 +5455,12 @@
       <c r="K95" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L95">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>54</v>
       </c>
@@ -4590,8 +5494,12 @@
       <c r="K96" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L96">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>54</v>
       </c>
@@ -4625,8 +5533,12 @@
       <c r="K97" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L97">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>54</v>
       </c>
@@ -4660,8 +5572,12 @@
       <c r="K98" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>54</v>
       </c>
@@ -4695,8 +5611,12 @@
       <c r="K99" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L99">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>58</v>
       </c>
@@ -4730,8 +5650,12 @@
       <c r="K100" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L100">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>58</v>
       </c>
@@ -4765,8 +5689,12 @@
       <c r="K101" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L101">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>58</v>
       </c>
@@ -4800,8 +5728,12 @@
       <c r="K102" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L102">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>58</v>
       </c>
@@ -4835,8 +5767,12 @@
       <c r="K103" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L103">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>58</v>
       </c>
@@ -4870,8 +5806,12 @@
       <c r="K104" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L104">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>58</v>
       </c>
@@ -4905,8 +5845,12 @@
       <c r="K105" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L105">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>58</v>
       </c>
@@ -4940,8 +5884,12 @@
       <c r="K106" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L106">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>61</v>
       </c>
@@ -4975,8 +5923,12 @@
       <c r="K107" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L107">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>61</v>
       </c>
@@ -5010,8 +5962,12 @@
       <c r="K108" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L108">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>61</v>
       </c>
@@ -5045,8 +6001,12 @@
       <c r="K109" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L109">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>61</v>
       </c>
@@ -5080,8 +6040,12 @@
       <c r="K110" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L110">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>61</v>
       </c>
@@ -5115,8 +6079,12 @@
       <c r="K111" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L111">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>61</v>
       </c>
@@ -5150,8 +6118,12 @@
       <c r="K112" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L112">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>61</v>
       </c>
@@ -5185,8 +6157,12 @@
       <c r="K113" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L113">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>63</v>
       </c>
@@ -5220,8 +6196,12 @@
       <c r="K114" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L114">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>63</v>
       </c>
@@ -5255,8 +6235,12 @@
       <c r="K115" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L115">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>63</v>
       </c>
@@ -5290,8 +6274,12 @@
       <c r="K116" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L116">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>63</v>
       </c>
@@ -5325,8 +6313,12 @@
       <c r="K117" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L117">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>68</v>
       </c>
@@ -5360,8 +6352,12 @@
       <c r="K118" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L118">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>68</v>
       </c>
@@ -5395,8 +6391,12 @@
       <c r="K119" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L119">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>68</v>
       </c>
@@ -5430,8 +6430,12 @@
       <c r="K120" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L120">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>68</v>
       </c>
@@ -5465,8 +6469,12 @@
       <c r="K121" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L121">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>68</v>
       </c>
@@ -5500,8 +6508,12 @@
       <c r="K122" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L122">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>68</v>
       </c>
@@ -5535,8 +6547,12 @@
       <c r="K123" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L123">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>68</v>
       </c>
@@ -5570,8 +6586,12 @@
       <c r="K124" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L124">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>71</v>
       </c>
@@ -5605,8 +6625,12 @@
       <c r="K125" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L125">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>71</v>
       </c>
@@ -5640,8 +6664,12 @@
       <c r="K126" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L126">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>71</v>
       </c>
@@ -5675,8 +6703,12 @@
       <c r="K127" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L127">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>71</v>
       </c>
@@ -5710,8 +6742,12 @@
       <c r="K128" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L128">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>71</v>
       </c>
@@ -5745,8 +6781,12 @@
       <c r="K129" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L129">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>77</v>
       </c>
@@ -5780,8 +6820,12 @@
       <c r="K130" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L130">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>77</v>
       </c>
@@ -5815,8 +6859,12 @@
       <c r="K131" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L131">
+        <f t="shared" ref="L131:L161" si="2">LEN(K131)/2</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>77</v>
       </c>
@@ -5850,8 +6898,12 @@
       <c r="K132" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L132">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>77</v>
       </c>
@@ -5885,8 +6937,12 @@
       <c r="K133" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L133">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>77</v>
       </c>
@@ -5920,8 +6976,12 @@
       <c r="K134" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L134">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>77</v>
       </c>
@@ -5955,8 +7015,12 @@
       <c r="K135" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L135">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>77</v>
       </c>
@@ -5990,8 +7054,12 @@
       <c r="K136" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L136">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>81</v>
       </c>
@@ -6025,8 +7093,12 @@
       <c r="K137" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L137">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>81</v>
       </c>
@@ -6060,8 +7132,12 @@
       <c r="K138" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L138">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>81</v>
       </c>
@@ -6095,8 +7171,12 @@
       <c r="K139" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L139">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>81</v>
       </c>
@@ -6130,8 +7210,12 @@
       <c r="K140" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L140">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>81</v>
       </c>
@@ -6165,8 +7249,12 @@
       <c r="K141" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L141">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>81</v>
       </c>
@@ -6200,8 +7288,12 @@
       <c r="K142" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L142">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>81</v>
       </c>
@@ -6235,8 +7327,12 @@
       <c r="K143" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L143">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>87</v>
       </c>
@@ -6270,8 +7366,12 @@
       <c r="K144" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L144">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>87</v>
       </c>
@@ -6305,8 +7405,12 @@
       <c r="K145" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L145">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>87</v>
       </c>
@@ -6340,8 +7444,12 @@
       <c r="K146" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L146">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>87</v>
       </c>
@@ -6375,8 +7483,12 @@
       <c r="K147" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L147">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>87</v>
       </c>
@@ -6410,8 +7522,12 @@
       <c r="K148" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L148">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>93</v>
       </c>
@@ -6445,8 +7561,12 @@
       <c r="K149" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L149">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>93</v>
       </c>
@@ -6480,8 +7600,12 @@
       <c r="K150" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L150">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>93</v>
       </c>
@@ -6515,8 +7639,12 @@
       <c r="K151" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L151">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>93</v>
       </c>
@@ -6550,8 +7678,12 @@
       <c r="K152" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L152">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>93</v>
       </c>
@@ -6585,8 +7717,12 @@
       <c r="K153" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L153">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>93</v>
       </c>
@@ -6620,8 +7756,12 @@
       <c r="K154" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L154">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>93</v>
       </c>
@@ -6655,8 +7795,12 @@
       <c r="K155" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L155">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>98</v>
       </c>
@@ -6690,8 +7834,12 @@
       <c r="K156" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L156">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>98</v>
       </c>
@@ -6725,8 +7873,12 @@
       <c r="K157" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L157">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>101</v>
       </c>
@@ -6760,8 +7912,12 @@
       <c r="K158" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L158">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>101</v>
       </c>
@@ -6795,8 +7951,12 @@
       <c r="K159" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L159">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>101</v>
       </c>
@@ -6830,8 +7990,12 @@
       <c r="K160" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L160">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="161" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>105</v>
       </c>
@@ -6865,8 +8029,12 @@
       <c r="K161" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L161">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>13</v>
       </c>
@@ -6882,19 +8050,34 @@
       <c r="G164" t="s">
         <v>119</v>
       </c>
-      <c r="I164" t="s">
-        <v>117</v>
-      </c>
-      <c r="J164" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K164" t="s">
+        <v>135</v>
+      </c>
+      <c r="L164" t="s">
+        <v>136</v>
+      </c>
+      <c r="N164" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>138</v>
+      </c>
+      <c r="R164" t="s">
+        <v>136</v>
+      </c>
+      <c r="T164" t="s">
+        <v>139</v>
+      </c>
+      <c r="U164" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>107</v>
       </c>
       <c r="B165">
-        <f>COUNTIF(B2:B161, "bfs")</f>
+        <f>COUNTIF($B$2:$B$161, "bfs")</f>
         <v>25</v>
       </c>
       <c r="C165">
@@ -6905,87 +8088,159 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="F165">
-        <f>SUMIFS($F2:$F161, B2:B161, "bfs")</f>
+        <f>SUMIFS($F2:$F161, $B$2:$B$161, "bfs")</f>
         <v>63162</v>
       </c>
       <c r="G165">
         <f>(F165 / B165)</f>
         <v>2526.48</v>
       </c>
-      <c r="I165">
-        <f>SUMIFS($G2:$G161, E2:E161, "bfs")</f>
-        <v>0</v>
-      </c>
-      <c r="J165" t="e">
-        <f>(I165 / E165)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K165">
+        <f>SUMIFS($H2:$H161, $B$2:$B$161, "bfs")</f>
+        <v>335</v>
+      </c>
+      <c r="L165">
+        <f>(K165 / $B$165)</f>
+        <v>13.4</v>
+      </c>
+      <c r="N165">
+        <f>SUMIFS($I2:$I161, $B$2:$B$161, "bfs")</f>
+        <v>18717</v>
+      </c>
+      <c r="O165">
+        <f>(N165 / $B$165)</f>
+        <v>748.68</v>
+      </c>
+      <c r="Q165">
+        <f>SUMIFS($J2:$J161, $B$2:$B$161, "bfs")</f>
+        <v>163.44187330700001</v>
+      </c>
+      <c r="R165">
+        <f>(Q165 / $B$165)</f>
+        <v>6.5376749322800007</v>
+      </c>
+      <c r="T165">
+        <f>SUMIFS($L2:$L161, $B$2:$B$161, "bfs")</f>
+        <v>859</v>
+      </c>
+      <c r="U165">
+        <f>(T165 / $B$165)</f>
+        <v>34.36</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>110</v>
       </c>
       <c r="B166">
-        <f>COUNTIFS(D2:D161, "Manhattan", E2:E161, "Fixed (1)")</f>
+        <f>COUNTIFS($D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (1)")</f>
         <v>21</v>
       </c>
       <c r="C166">
         <v>30</v>
       </c>
       <c r="D166" s="1">
-        <f>((B166/C166) )</f>
+        <f t="shared" ref="D166:D171" si="3">((B166/C166) )</f>
         <v>0.7</v>
       </c>
       <c r="F166">
-        <f>SUMIFS($F2:$F161, D2:D161, "Manhattan", E2:E161, "Fixed (1)")</f>
+        <f>SUMIFS($F2:$F$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (1)")</f>
         <v>6263</v>
       </c>
       <c r="G166">
         <f>(F166 / B166)</f>
         <v>298.23809523809524</v>
       </c>
-      <c r="I166">
-        <f>SUMIFS($F2:$F161, G2:G161, "Manhattan", H2:H161, "Fixed (1)")</f>
-        <v>0</v>
-      </c>
-      <c r="J166" t="e">
-        <f>(I166 / E166)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K166">
+        <f>SUMIFS($H2:$H$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (1)")</f>
+        <v>1719</v>
+      </c>
+      <c r="L166">
+        <f t="shared" ref="L166:L171" si="4">(K166 / $B$165)</f>
+        <v>68.760000000000005</v>
+      </c>
+      <c r="N166">
+        <f>SUMIFS($I2:$I$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (1)")</f>
+        <v>34715</v>
+      </c>
+      <c r="O166">
+        <f t="shared" ref="O166:O171" si="5">(N166 / $B$165)</f>
+        <v>1388.6</v>
+      </c>
+      <c r="Q166">
+        <f>SUMIFS($J2:$J$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (1)")</f>
+        <v>173.443422328</v>
+      </c>
+      <c r="R166">
+        <f t="shared" ref="R166:R171" si="6">(Q166 / $B$165)</f>
+        <v>6.9377368931200003</v>
+      </c>
+      <c r="T166">
+        <f>SUMIFS($L2:$L$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (1)")</f>
+        <v>470</v>
+      </c>
+      <c r="U166">
+        <f t="shared" ref="U166:U171" si="7">(T166 / $B$165)</f>
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>111</v>
       </c>
       <c r="B167">
-        <f>COUNTIFS(D2:D161, "Manhattan", E2:E161, "Fixed (4)")</f>
+        <f>COUNTIFS($D2:D161, "Manhattan", E2:E161, "Fixed (4)")</f>
         <v>26</v>
       </c>
       <c r="C167">
         <v>30</v>
       </c>
       <c r="D167" s="1">
-        <f>((B167/C167) )</f>
+        <f t="shared" si="3"/>
         <v>0.8666666666666667</v>
       </c>
       <c r="F167">
-        <f t="shared" ref="F166:F171" si="0">SUMIFS($F4:$F163, B4:B163, "bfs")</f>
-        <v>63160</v>
+        <f>SUMIFS($F$2:$F$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (4)")</f>
+        <v>28666</v>
       </c>
       <c r="G167">
         <f>(F167 / B167)</f>
-        <v>2429.2307692307691</v>
-      </c>
-      <c r="I167">
-        <f t="shared" ref="I167:I171" si="1">SUMIFS($F4:$F163, E4:E163, "bfs")</f>
-        <v>0</v>
-      </c>
-      <c r="J167" t="e">
-        <f>(I167 / E167)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1102.5384615384614</v>
+      </c>
+      <c r="K167">
+        <f>SUMIFS($H$2:$H$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (4)")</f>
+        <v>5564</v>
+      </c>
+      <c r="L167">
+        <f t="shared" si="4"/>
+        <v>222.56</v>
+      </c>
+      <c r="N167">
+        <f>SUMIFS($I$2:$I$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (4)")</f>
+        <v>69785</v>
+      </c>
+      <c r="O167">
+        <f t="shared" si="5"/>
+        <v>2791.4</v>
+      </c>
+      <c r="Q167">
+        <f>SUMIFS($J$2:$J$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (4)")</f>
+        <v>459.18132976999999</v>
+      </c>
+      <c r="R167">
+        <f t="shared" si="6"/>
+        <v>18.3672531908</v>
+      </c>
+      <c r="T167">
+        <f>SUMIFS($L$2:$L$161, $D$2:$D$161, "Manhattan", $E$2:$E$161, "Fixed (4)")</f>
+        <v>666</v>
+      </c>
+      <c r="U167">
+        <f t="shared" si="7"/>
+        <v>26.64</v>
+      </c>
+    </row>
+    <row r="168" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>112</v>
       </c>
@@ -6997,27 +8252,51 @@
         <v>30</v>
       </c>
       <c r="D168" s="1">
-        <f>((B168/C168) )</f>
+        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
       <c r="F168">
-        <f t="shared" si="0"/>
-        <v>63160</v>
+        <f>SUMIFS($F$2:$F$161, $D$2:$D$161, "Manhattan", $E$4:$E$163, "Dynamic")</f>
+        <v>13765</v>
       </c>
       <c r="G168">
         <f>(F168 / B168)</f>
-        <v>2631.6666666666665</v>
-      </c>
-      <c r="I168">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J168" t="e">
-        <f>(I168 / E168)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+        <v>573.54166666666663</v>
+      </c>
+      <c r="K168">
+        <f>SUMIFS($H$2:$H$161, $D$2:$D$161, "Manhattan", $E$4:$E$163, "Dynamic")</f>
+        <v>3600</v>
+      </c>
+      <c r="L168">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="N168">
+        <f>SUMIFS($I$2:$I$161, $D$2:$D$161, "Manhattan", $E$4:$E$163, "Dynamic")</f>
+        <v>55687</v>
+      </c>
+      <c r="O168">
+        <f t="shared" si="5"/>
+        <v>2227.48</v>
+      </c>
+      <c r="Q168">
+        <f>SUMIFS($J$2:$J$161, $D$2:$D$161, "Manhattan", $E$4:$E$163, "Dynamic")</f>
+        <v>314.17527223799999</v>
+      </c>
+      <c r="R168">
+        <f t="shared" si="6"/>
+        <v>12.567010889519999</v>
+      </c>
+      <c r="T168">
+        <f>SUMIFS($L$2:$L$161, $D$2:$D$161, "Manhattan", $E$4:$E$163, "Dynamic")</f>
+        <v>532</v>
+      </c>
+      <c r="U168">
+        <f t="shared" si="7"/>
+        <v>21.28</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>113</v>
       </c>
@@ -7029,27 +8308,51 @@
         <v>30</v>
       </c>
       <c r="D169" s="1">
-        <f>((B169/C169) )</f>
+        <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="F169">
-        <f t="shared" si="0"/>
-        <v>63160</v>
+      <c r="F169" s="28">
+        <f>SUMIFS($F$2:$F$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (1)")</f>
+        <v>3789</v>
       </c>
       <c r="G169">
         <f>(F169 / B169)</f>
-        <v>3158</v>
-      </c>
-      <c r="I169">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J169" t="e">
-        <f>(I169 / E169)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+        <v>189.45</v>
+      </c>
+      <c r="K169" s="28">
+        <f>SUMIFS($H$2:$H$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (1)")</f>
+        <v>2621</v>
+      </c>
+      <c r="L169">
+        <f t="shared" si="4"/>
+        <v>104.84</v>
+      </c>
+      <c r="N169" s="28">
+        <f>SUMIFS($I$2:$I$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (1)")</f>
+        <v>43976</v>
+      </c>
+      <c r="O169">
+        <f t="shared" si="5"/>
+        <v>1759.04</v>
+      </c>
+      <c r="Q169" s="28">
+        <f>SUMIFS($J$2:$J$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (1)")</f>
+        <v>206.20237756000003</v>
+      </c>
+      <c r="R169">
+        <f t="shared" si="6"/>
+        <v>8.2480951024000007</v>
+      </c>
+      <c r="T169" s="28">
+        <f>SUMIFS($L$2:$L$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (1)")</f>
+        <v>436</v>
+      </c>
+      <c r="U169">
+        <f t="shared" si="7"/>
+        <v>17.440000000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>114</v>
       </c>
@@ -7061,27 +8364,51 @@
         <v>30</v>
       </c>
       <c r="D170" s="1">
-        <f>((B170/C170) )</f>
+        <f t="shared" si="3"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="F170">
-        <f t="shared" si="0"/>
-        <v>63160</v>
+      <c r="F170" s="28">
+        <f>SUMIFS($F$2:$F$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (4)")</f>
+        <v>11278</v>
       </c>
       <c r="G170">
-        <f t="shared" ref="G168:G171" si="2">(F170 / B170)</f>
-        <v>2746.086956521739</v>
-      </c>
-      <c r="I170">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J170" t="e">
-        <f t="shared" ref="J170:J171" si="3">(I170 / E170)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G170:G171" si="8">(F170 / B170)</f>
+        <v>490.3478260869565</v>
+      </c>
+      <c r="K170" s="28">
+        <f>SUMIFS($H$2:$H$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (4)")</f>
+        <v>2393</v>
+      </c>
+      <c r="L170">
+        <f t="shared" si="4"/>
+        <v>95.72</v>
+      </c>
+      <c r="N170" s="28">
+        <f>SUMIFS($I$2:$I$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (4)")</f>
+        <v>40416</v>
+      </c>
+      <c r="O170">
+        <f t="shared" si="5"/>
+        <v>1616.64</v>
+      </c>
+      <c r="Q170" s="28">
+        <f>SUMIFS($J$2:$J$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (4)")</f>
+        <v>237.52572703300001</v>
+      </c>
+      <c r="R170">
+        <f t="shared" si="6"/>
+        <v>9.5010290813200005</v>
+      </c>
+      <c r="T170" s="28">
+        <f>SUMIFS($L$2:$L$161, $D$2:$D$161, "Euclidean", $E$2:$E$161, "Fixed (4)")</f>
+        <v>569</v>
+      </c>
+      <c r="U170">
+        <f t="shared" si="7"/>
+        <v>22.76</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>115</v>
       </c>
@@ -7093,105 +8420,946 @@
         <v>30</v>
       </c>
       <c r="D171" s="1">
-        <f>((B171/C171) )</f>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="F171">
-        <f t="shared" si="0"/>
-        <v>63160</v>
+      <c r="F171" s="28">
+        <f>SUMIFS($F$2:$F$161, $D$2:$D$161, "Euclidean", $E$3:$E$162, "Dynamic")</f>
+        <v>7602</v>
       </c>
       <c r="G171">
-        <f t="shared" si="2"/>
-        <v>3007.6190476190477</v>
-      </c>
-      <c r="I171">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J171" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F173" t="s">
-        <v>120</v>
-      </c>
-      <c r="G173" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F174">
-        <f>SUMIFS($F11:$F170, B11:B170, "bfs")</f>
-        <v>63158</v>
-      </c>
-      <c r="G174" t="e">
-        <f>(F174 / B174)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F175">
-        <f>SUMIFS($F11:$F170, D11:D170, "Manhattan", E11:E170, "Fixed (1)")</f>
-        <v>6259</v>
-      </c>
-      <c r="G175" t="e">
-        <f>(F175 / B175)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F176">
-        <f t="shared" ref="F176:F180" si="4">SUMIFS($F13:$F172, B13:B172, "bfs")</f>
-        <v>63158</v>
-      </c>
-      <c r="G176" t="e">
-        <f>(F176 / B176)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="177" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F177">
+        <f t="shared" si="8"/>
+        <v>362</v>
+      </c>
+      <c r="K171" s="28">
+        <f>SUMIFS($H$2:$H$161, $D$2:$D$161, "Euclidean", $E$3:$E$162, "Dynamic")</f>
+        <v>1471</v>
+      </c>
+      <c r="L171">
         <f t="shared" si="4"/>
-        <v>63158</v>
-      </c>
-      <c r="G177" t="e">
-        <f>(F177 / B177)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="178" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F178">
-        <f t="shared" si="4"/>
-        <v>63158</v>
-      </c>
-      <c r="G178" t="e">
-        <f>(F178 / B178)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="179" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F179">
-        <f t="shared" si="4"/>
-        <v>63158</v>
-      </c>
-      <c r="G179" t="e">
-        <f t="shared" ref="G179:G180" si="5">(F179 / B179)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="180" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F180">
-        <f t="shared" si="4"/>
-        <v>63142</v>
-      </c>
-      <c r="G180" t="e">
+        <v>58.84</v>
+      </c>
+      <c r="N171" s="28">
+        <f>SUMIFS($I$2:$I$161, $D$2:$D$161, "Euclidean", $E$3:$E$162, "Dynamic")</f>
+        <v>24548</v>
+      </c>
+      <c r="O171">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>981.92</v>
+      </c>
+      <c r="Q171" s="28">
+        <f>SUMIFS($J$2:$J$161, $D$2:$D$161, "Euclidean", $E$3:$E$162, "Dynamic")</f>
+        <v>139.05307888599998</v>
+      </c>
+      <c r="R171">
+        <f t="shared" si="6"/>
+        <v>5.5621231554399992</v>
+      </c>
+      <c r="T171" s="28">
+        <f>SUMIFS($L$2:$L$161, $D$2:$D$161, "Euclidean", $E$3:$E$162, "Dynamic")</f>
+        <v>519</v>
+      </c>
+      <c r="U171">
+        <f t="shared" si="7"/>
+        <v>20.76</v>
+      </c>
+    </row>
+    <row r="176" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="I176" t="s">
+        <v>117</v>
+      </c>
+      <c r="J176" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="177" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I177">
+        <f>SUMIFS($G2:$G161, E2:E161, "bfs")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I178">
+        <f>SUMIFS($F2:$F161, G2:G161, "Manhattan", H2:H161, "Fixed (1)")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I179">
+        <f>SUMIFS($F4:$F163, E4:E163, "bfs")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I180">
+        <f>SUMIFS($F5:$F164, E5:E164, "bfs")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I181">
+        <f>SUMIFS($F6:$F165, E6:E165, "bfs")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I182">
+        <f>SUMIFS($F7:$F166, E7:E166, "bfs")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I183">
+        <f>SUMIFS($F8:$F167, E8:E167, "bfs")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7A9E83-ACF7-2C48-AF62-F87EA40ABD55}">
+  <dimension ref="B1:O23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="36"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="31">
+        <v>27</v>
+      </c>
+      <c r="D5" s="15">
+        <v>30</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="14">
+        <v>16413</v>
+      </c>
+      <c r="G5" s="17">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="H5" s="14">
+        <v>3096</v>
+      </c>
+      <c r="I5" s="17">
+        <v>114.66666666666667</v>
+      </c>
+      <c r="J5" s="14">
+        <v>70217</v>
+      </c>
+      <c r="K5" s="17">
+        <v>2600.6296296296296</v>
+      </c>
+      <c r="L5" s="18">
+        <v>347.98502039909312</v>
+      </c>
+      <c r="M5" s="17">
+        <v>12.8883340888553</v>
+      </c>
+      <c r="N5" s="14">
+        <v>1304</v>
+      </c>
+      <c r="O5" s="19">
+        <v>48.296296296296298</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B6" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="14">
+        <v>19</v>
+      </c>
+      <c r="D6" s="15">
+        <v>30</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="F6" s="14">
+        <v>9142</v>
+      </c>
+      <c r="G6" s="17">
+        <v>481.15789473684208</v>
+      </c>
+      <c r="H6" s="14">
+        <v>2163</v>
+      </c>
+      <c r="I6" s="17">
+        <v>113.84210526315789</v>
+      </c>
+      <c r="J6" s="14">
+        <v>73463</v>
+      </c>
+      <c r="K6" s="17">
+        <v>3866.4736842105262</v>
+      </c>
+      <c r="L6" s="18">
+        <v>313.71195602416947</v>
+      </c>
+      <c r="M6" s="17">
+        <v>16.511155580219445</v>
+      </c>
+      <c r="N6" s="14">
+        <v>678</v>
+      </c>
+      <c r="O6" s="30">
+        <v>35.684210526315802</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="14">
+        <v>21</v>
+      </c>
+      <c r="D7" s="15">
+        <v>30</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="14">
+        <v>11117</v>
+      </c>
+      <c r="G7" s="17">
+        <v>529.38095238095241</v>
+      </c>
+      <c r="H7" s="14">
+        <v>1814</v>
+      </c>
+      <c r="I7" s="17">
+        <v>86.38095238095238</v>
+      </c>
+      <c r="J7" s="14">
+        <v>52067</v>
+      </c>
+      <c r="K7" s="17">
+        <v>2479.3809523809523</v>
+      </c>
+      <c r="L7" s="18">
+        <v>254.65401196479749</v>
+      </c>
+      <c r="M7" s="29">
+        <v>12.126381522133213</v>
+      </c>
+      <c r="N7" s="14">
+        <v>901</v>
+      </c>
+      <c r="O7" s="19">
+        <v>42.904761904761905</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="14">
+        <v>19</v>
+      </c>
+      <c r="D8" s="15">
+        <v>30</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="F8" s="14">
+        <v>10135</v>
+      </c>
+      <c r="G8" s="17">
+        <v>533.42105263157896</v>
+      </c>
+      <c r="H8" s="14">
+        <v>2241</v>
+      </c>
+      <c r="I8" s="17">
+        <v>117.94736842105263</v>
+      </c>
+      <c r="J8" s="14">
+        <v>65918</v>
+      </c>
+      <c r="K8" s="17">
+        <v>3469.3684210526317</v>
+      </c>
+      <c r="L8" s="18">
+        <v>296.80949282646122</v>
+      </c>
+      <c r="M8" s="17">
+        <v>15.621552254024275</v>
+      </c>
+      <c r="N8" s="14">
+        <v>700</v>
+      </c>
+      <c r="O8" s="19">
+        <v>36.842105263157897</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="14">
+        <v>12</v>
+      </c>
+      <c r="D9" s="15">
+        <v>30</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="14">
+        <v>6030</v>
+      </c>
+      <c r="G9" s="17">
+        <v>502.5</v>
+      </c>
+      <c r="H9" s="14">
+        <v>1877</v>
+      </c>
+      <c r="I9" s="17">
+        <v>156.41666666666666</v>
+      </c>
+      <c r="J9" s="14">
+        <v>54073</v>
+      </c>
+      <c r="K9" s="17">
+        <v>4506.083333333333</v>
+      </c>
+      <c r="L9" s="18">
+        <v>220.85452294349639</v>
+      </c>
+      <c r="M9" s="17">
+        <v>18.4045435786247</v>
+      </c>
+      <c r="N9" s="14">
+        <v>391</v>
+      </c>
+      <c r="O9" s="20">
+        <v>32.583333333333336</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="14">
+        <v>21</v>
+      </c>
+      <c r="D10" s="15">
+        <v>30</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="F10" s="14">
+        <v>11569</v>
+      </c>
+      <c r="G10" s="17">
+        <v>550.90476190476193</v>
+      </c>
+      <c r="H10" s="14">
+        <v>1942</v>
+      </c>
+      <c r="I10" s="17">
+        <v>92.476190476190482</v>
+      </c>
+      <c r="J10" s="14">
+        <v>61388</v>
+      </c>
+      <c r="K10" s="17">
+        <v>2923.2380952380954</v>
+      </c>
+      <c r="L10" s="18">
+        <v>305.465868234634</v>
+      </c>
+      <c r="M10" s="17">
+        <v>14.545993725458763</v>
+      </c>
+      <c r="N10" s="14">
+        <v>866</v>
+      </c>
+      <c r="O10" s="19">
+        <v>41.238095238095241</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="22">
+        <v>14</v>
+      </c>
+      <c r="D11" s="23">
+        <v>30</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="F11" s="22">
+        <v>8037</v>
+      </c>
+      <c r="G11" s="25">
+        <v>574.07142857142856</v>
+      </c>
+      <c r="H11" s="22">
+        <v>2710</v>
+      </c>
+      <c r="I11" s="25">
+        <v>193.57142857142858</v>
+      </c>
+      <c r="J11" s="22">
+        <v>67637</v>
+      </c>
+      <c r="K11" s="25">
+        <v>4831.2142857142853</v>
+      </c>
+      <c r="L11" s="26">
+        <v>288.99031686782808</v>
+      </c>
+      <c r="M11" s="25">
+        <v>20.642165490559147</v>
+      </c>
+      <c r="N11" s="22">
+        <v>477</v>
+      </c>
+      <c r="O11" s="27">
+        <v>34.071428571428569</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:15" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="14">
+        <v>25</v>
+      </c>
+      <c r="D17" s="15">
+        <v>30</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F17" s="14">
+        <v>63162</v>
+      </c>
+      <c r="G17" s="17">
+        <v>2526.48</v>
+      </c>
+      <c r="H17" s="14">
+        <v>335</v>
+      </c>
+      <c r="I17" s="17">
+        <v>13.4</v>
+      </c>
+      <c r="J17" s="14">
+        <v>18717</v>
+      </c>
+      <c r="K17" s="17">
+        <v>748.68</v>
+      </c>
+      <c r="L17" s="18">
+        <v>163.44187330700001</v>
+      </c>
+      <c r="M17" s="17">
+        <v>6.5376749322800007</v>
+      </c>
+      <c r="N17" s="14">
+        <v>859</v>
+      </c>
+      <c r="O17" s="19">
+        <v>34.36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B18" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="14">
+        <v>21</v>
+      </c>
+      <c r="D18" s="15">
+        <v>30</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="F18" s="14">
+        <v>6263</v>
+      </c>
+      <c r="G18" s="17">
+        <v>298.23809523809524</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1719</v>
+      </c>
+      <c r="I18" s="17">
+        <v>68.760000000000005</v>
+      </c>
+      <c r="J18" s="14">
+        <v>34715</v>
+      </c>
+      <c r="K18" s="17">
+        <v>1388.6</v>
+      </c>
+      <c r="L18" s="18">
+        <v>173.443422328</v>
+      </c>
+      <c r="M18" s="17">
+        <v>6.9377368931200003</v>
+      </c>
+      <c r="N18" s="14">
+        <v>470</v>
+      </c>
+      <c r="O18" s="30">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="31">
+        <v>26</v>
+      </c>
+      <c r="D19" s="15">
+        <v>30</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="F19" s="14">
+        <v>28666</v>
+      </c>
+      <c r="G19" s="17">
+        <v>1102.5384615384614</v>
+      </c>
+      <c r="H19" s="14">
+        <v>5564</v>
+      </c>
+      <c r="I19" s="17">
+        <v>222.56</v>
+      </c>
+      <c r="J19" s="14">
+        <v>69785</v>
+      </c>
+      <c r="K19" s="17">
+        <v>2791.4</v>
+      </c>
+      <c r="L19" s="18">
+        <v>459.18132976999999</v>
+      </c>
+      <c r="M19" s="17">
+        <v>18.3672531908</v>
+      </c>
+      <c r="N19" s="14">
+        <v>666</v>
+      </c>
+      <c r="O19" s="19">
+        <v>26.64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="14">
+        <v>24</v>
+      </c>
+      <c r="D20" s="15">
+        <v>30</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="14">
+        <v>13765</v>
+      </c>
+      <c r="G20" s="17">
+        <v>573.54166666666663</v>
+      </c>
+      <c r="H20" s="14">
+        <v>3600</v>
+      </c>
+      <c r="I20" s="17">
+        <v>144</v>
+      </c>
+      <c r="J20" s="14">
+        <v>55687</v>
+      </c>
+      <c r="K20" s="17">
+        <v>2227.48</v>
+      </c>
+      <c r="L20" s="18">
+        <v>314.17527223799999</v>
+      </c>
+      <c r="M20" s="32">
+        <v>12.567010889519999</v>
+      </c>
+      <c r="N20" s="14">
+        <v>532</v>
+      </c>
+      <c r="O20" s="19">
+        <v>21.28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="14">
+        <v>20</v>
+      </c>
+      <c r="D21" s="15">
+        <v>30</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F21" s="14">
+        <v>3789</v>
+      </c>
+      <c r="G21" s="17">
+        <v>189.45</v>
+      </c>
+      <c r="H21" s="14">
+        <v>2621</v>
+      </c>
+      <c r="I21" s="17">
+        <v>104.84</v>
+      </c>
+      <c r="J21" s="14">
+        <v>43976</v>
+      </c>
+      <c r="K21" s="17">
+        <v>1759.04</v>
+      </c>
+      <c r="L21" s="18">
+        <v>206.20237756000003</v>
+      </c>
+      <c r="M21" s="17">
+        <v>8.2480951024000007</v>
+      </c>
+      <c r="N21" s="14">
+        <v>436</v>
+      </c>
+      <c r="O21" s="20">
+        <v>17.440000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="14">
+        <v>23</v>
+      </c>
+      <c r="D22" s="15">
+        <v>30</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0.76666666666666672</v>
+      </c>
+      <c r="F22" s="14">
+        <v>11278</v>
+      </c>
+      <c r="G22" s="17">
+        <v>490.3478260869565</v>
+      </c>
+      <c r="H22" s="14">
+        <v>2393</v>
+      </c>
+      <c r="I22" s="17">
+        <v>95.72</v>
+      </c>
+      <c r="J22" s="14">
+        <v>40416</v>
+      </c>
+      <c r="K22" s="17">
+        <v>1616.64</v>
+      </c>
+      <c r="L22" s="18">
+        <v>237.52572703300001</v>
+      </c>
+      <c r="M22" s="17">
+        <v>9.5010290813200005</v>
+      </c>
+      <c r="N22" s="14">
+        <v>569</v>
+      </c>
+      <c r="O22" s="19">
+        <v>22.76</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="22">
+        <v>21</v>
+      </c>
+      <c r="D23" s="23">
+        <v>30</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="F23" s="22">
+        <v>7602</v>
+      </c>
+      <c r="G23" s="25">
+        <v>362</v>
+      </c>
+      <c r="H23" s="22">
+        <v>1471</v>
+      </c>
+      <c r="I23" s="25">
+        <v>58.84</v>
+      </c>
+      <c r="J23" s="22">
+        <v>24548</v>
+      </c>
+      <c r="K23" s="25">
+        <v>981.92</v>
+      </c>
+      <c r="L23" s="26">
+        <v>139.05307888599998</v>
+      </c>
+      <c r="M23" s="33">
+        <v>5.5621231554399992</v>
+      </c>
+      <c r="N23" s="22">
+        <v>519</v>
+      </c>
+      <c r="O23" s="27">
+        <v>20.76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D550E3D1-1E7E-5748-B62C-46303C274094}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>